<commit_message>
now all the mode showhint load from excel sheet
</commit_message>
<xml_diff>
--- a/app/src/main/assets/hint/en.xlsx
+++ b/app/src/main/assets/hint/en.xlsx
@@ -1,30 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29012"/>
-  <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C0BA3A4-EB7E-4B46-AD00-441D6FDC48AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -33,16 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t>mode</t>
-  </si>
-  <si>
-    <t>hint</t>
-  </si>
-  <si>
-    <t>quickplay</t>
-  </si>
-  <si>
-    <t>Welcome to the  This Mode ! This game helps you practice adding numbers with clear spoken questions.
+    <t xml:space="preserve">mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quickplay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to the  This Mode ! This game helps you practice adding numbers with clear spoken questions.
 Objective of the Game
 You will hear or see a story problem . Your task is to find the total sum of two numbers and enter the correct answer.
 Gameplay Instructions
@@ -57,7 +46,7 @@
 Buttons are labeled for screen readers."</t>
   </si>
   <si>
-    <t>shake</t>
+    <t xml:space="preserve">shake</t>
   </si>
   <si>
     <t xml:space="preserve">This game tests your ability to shake your device a specified number of times as fast as possible while listening to voice instructions and receiving feedback.
@@ -111,7 +100,7 @@
 </t>
   </si>
   <si>
-    <t>tap</t>
+    <t xml:space="preserve">tap</t>
   </si>
   <si>
     <t xml:space="preserve">This game challenges you to tap the screen a specific number of times as indicated by a simple math expression. You’ll receive spoken instructions and audio feedback throughout.
@@ -162,10 +151,10 @@
 </t>
   </si>
   <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>How to Play:
+    <t xml:space="preserve">day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to Play:
 Welcome to the day guessing game!
 Here, you will hear a day of the week, like Monday or Friday, and a number telling you how many days to count forward.
 Your job is to figure out which day comes after adding those days.
@@ -175,10 +164,10 @@
 Try your best to answer as many questions as you can and watch yourself become a day master! Have fun, keep guessing, and enjoy learning the days of the week in a super fun way!</t>
   </si>
   <si>
-    <t>number line</t>
-  </si>
-  <si>
-    <t>Welcome to the Number Line Game! This game helps you practice addition and subtraction by moving along a number line using simple voice commands and button controls. Here’s a detailed guide to help you play:
+    <t xml:space="preserve">numberline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to the Number Line Game! This game helps you practice addition and subtraction by moving along a number line using simple voice commands and button controls. Here’s a detailed guide to help you play:
 Objective of the Game
 Your goal is to start at a certain position on an imaginary number line and move either left (subtract) or right (add) by a certain number of units to reach the correct final position.
 Game Setup
@@ -219,10 +208,10 @@
 Confused about position: Tap the question text to hear your current task again.</t>
   </si>
   <si>
-    <t>mind</t>
-  </si>
-  <si>
-    <t>Welcome to the Mental Calculation Game! This game tests your quick math skills by asking you to solve arithmetic problems spoken aloud. Here is a step-by-step guide to help you enjoy and succeed in the game using voice feedback and accessible controls.
+    <t xml:space="preserve">mental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to the Mental Calculation Game! This game tests your quick math skills by asking you to solve arithmetic problems spoken aloud. Here is a step-by-step guide to help you enjoy and succeed in the game using voice feedback and accessible controls.
 Objective of the Game
 Your goal is to listen carefully to the arithmetic problem spoken by the game and then enter the correct answer using the keyboard. The game will tell you if your answer is right or wrong, and you will advance through a series of questions.
 Game Setup
@@ -262,10 +251,10 @@
 Invalid Answer Warning: Enter only numbers without spaces or symbols. If you make a mistake, clear the input and try again.</t>
   </si>
   <si>
-    <t>angle</t>
-  </si>
-  <si>
-    <t>Welcome to the Angle Game, an exciting challenge where you will be asked to turn to specific angles using your device’s rotation sensors. Here's a detailed step-by-step guide to help you play the game:
+    <t xml:space="preserve">angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to the Angle Game, an exciting challenge where you will be asked to turn to specific angles using your device’s rotation sensors. Here's a detailed step-by-step guide to help you play the game:
 Objective of the Game
 Your goal is to correctly adjust the orientation of your device to match the target angle displayed in the game. You will receive verbal prompts to help guide you in turning the device to the correct angle.
 Game Setup
@@ -321,7 +310,7 @@
 If the device’s sensor isn’t responding well to your movements, try rotating your device slowly and steadily. Avoid sharp, quick turns.</t>
   </si>
   <si>
-    <t>echo</t>
+    <t xml:space="preserve">sterio</t>
   </si>
   <si>
     <t xml:space="preserve">Welcome to the Stereo Number Game! This game helps you practice subtraction using special stereo audio cues and speech. Here’s how to play:
@@ -359,7 +348,7 @@
 </t>
   </si>
   <si>
-    <t>sketch</t>
+    <t xml:space="preserve">drawing</t>
   </si>
   <si>
     <t xml:space="preserve">✏️ Welcome to the Drawing Game
@@ -420,7 +409,7 @@
 </t>
   </si>
   <si>
-    <t>path</t>
+    <t xml:space="preserve">compass</t>
   </si>
   <si>
     <t xml:space="preserve">🧭 Welcome to the Compass Game
@@ -492,7 +481,7 @@
 </t>
   </si>
   <si>
-    <t>touch</t>
+    <t xml:space="preserve">touch</t>
   </si>
   <si>
     <t xml:space="preserve">Welcome to the Touch Screen Game! This game helps you practice basic arithmetic by touching the screen with the correct number of fingers as your answer. Here’s how to play:
@@ -538,14 +527,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -557,7 +564,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -565,451 +572,160 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="0E2841"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="145F82"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="E87331"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="186C24"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="A02B93"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="4EA72E"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="467886"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="96607D"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="225.5703125" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="225.57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="346.5">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="346.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.6">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="115.5">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="115.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="409.6">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="409.6">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="409.6">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="409.6">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="409.6">
-      <c r="A10" t="s">
+    <row r="10" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="409.6">
-      <c r="A11" t="s">
+    <row r="11" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="409.6">
-      <c r="A12" t="s">
+    <row r="12" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1017,6 +733,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>